<commit_message>
MI & IL figures for RMI
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/parameters.xlsx
+++ b/state_fact_sheets/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmariano/Library/CloudStorage/Dropbox/1 Projects/Industrial-decarb/state_fact_sheets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3918F00-9E21-AE44-B9C6-1EE87F326633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA95E701-92A2-9942-B2C2-5A95EB61746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="500" windowWidth="25000" windowHeight="21100" xr2:uid="{3E12E361-6825-0D47-A000-BC6313A11324}"/>
+    <workbookView xWindow="19280" yWindow="520" windowWidth="19120" windowHeight="21100" xr2:uid="{3E12E361-6825-0D47-A000-BC6313A11324}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>scenario</t>
   </si>
@@ -82,16 +82,49 @@
   </si>
   <si>
     <t xml:space="preserve">$ per mmbtu </t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eia.gov/dnav/ng/ng_pri_sum_a_EPG0_PIN_DMcf_a.htm </t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/electricity/data/browser/#/topic/7?agg=1,0&amp;geo=vvvvvvvvvvvvo&amp;endsec=2&amp;freq=A&amp;start=2001&amp;end=2024&amp;ctype=linechart&amp;ltype=pin&amp;rtype=s&amp;maptype=0&amp;rse=0&amp;pin=</t>
+  </si>
+  <si>
+    <t>use filters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,13 +147,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4414B5-B70F-1948-892C-2F71AAC0B49C}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +544,7 @@
         <v>30</v>
       </c>
       <c r="D2">
-        <v>9.4600000000000004E-2</v>
+        <v>9.1399999999999995E-2</v>
       </c>
       <c r="E2">
         <v>5.37</v>
@@ -528,6 +565,76 @@
         <v>0.01</v>
       </c>
       <c r="K2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>8.2699999999999996E-2</v>
+      </c>
+      <c r="E3">
+        <v>7.57</v>
+      </c>
+      <c r="F3">
+        <v>0.03</v>
+      </c>
+      <c r="G3">
+        <v>0.06</v>
+      </c>
+      <c r="H3">
+        <v>0.01</v>
+      </c>
+      <c r="I3">
+        <v>0.01</v>
+      </c>
+      <c r="J3">
+        <v>0.01</v>
+      </c>
+      <c r="K3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -538,36 +645,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C481BB-55D0-CE45-8845-56FAAD0C5B2A}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{C7FCCB93-604B-8448-B1D1-6A2EE1CD9792}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementing fuel price projections for LCOH
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/parameters.xlsx
+++ b/state_fact_sheets/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmariano/Library/CloudStorage/Dropbox/1 Projects/Industrial-decarb/state_fact_sheets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA95E701-92A2-9942-B2C2-5A95EB61746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF8C5E1-1B2E-C443-AC7B-2A593438D65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="520" windowWidth="19120" windowHeight="21100" xr2:uid="{3E12E361-6825-0D47-A000-BC6313A11324}"/>
+    <workbookView xWindow="13040" yWindow="1860" windowWidth="25360" windowHeight="18380" xr2:uid="{3E12E361-6825-0D47-A000-BC6313A11324}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>scenario</t>
   </si>
@@ -54,33 +54,12 @@
     <t>ng_price</t>
   </si>
   <si>
-    <t>ngboiler_om_high</t>
-  </si>
-  <si>
-    <t>ngboiler_om_low</t>
-  </si>
-  <si>
-    <t>eboiler_om_high</t>
-  </si>
-  <si>
-    <t>eboiler_om_low</t>
-  </si>
-  <si>
-    <t>hthp_om_high</t>
-  </si>
-  <si>
-    <t>hthp_om_low</t>
-  </si>
-  <si>
     <t>MN</t>
   </si>
   <si>
     <t>Units</t>
   </si>
   <si>
-    <t>cents per kwh</t>
-  </si>
-  <si>
     <t xml:space="preserve">$ per mmbtu </t>
   </si>
   <si>
@@ -100,6 +79,33 @@
   </si>
   <si>
     <t>use filters</t>
+  </si>
+  <si>
+    <t>ngboiler_om_best</t>
+  </si>
+  <si>
+    <t>ngboiler_om_worst</t>
+  </si>
+  <si>
+    <t>eboiler_om_best</t>
+  </si>
+  <si>
+    <t>eboiler_om_worst</t>
+  </si>
+  <si>
+    <t>hthp_om_best</t>
+  </si>
+  <si>
+    <t>hthp_om_worst</t>
+  </si>
+  <si>
+    <t>$ per kWh</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4414B5-B70F-1948-892C-2F71AAC0B49C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,27 +521,27 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>6.5000000000000002E-2</v>
@@ -570,7 +576,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>6.5000000000000002E-2</v>
@@ -605,7 +611,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>6.5000000000000002E-2</v>
@@ -635,6 +641,41 @@
         <v>0.01</v>
       </c>
       <c r="K4" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.5199999999999998E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.76</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -645,7 +686,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C481BB-55D0-CE45-8845-56FAAD0C5B2A}">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -654,45 +695,55 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>2024</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>2024</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{C7FCCB93-604B-8448-B1D1-6A2EE1CD9792}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{C7FCCB93-604B-8448-B1D1-6A2EE1CD9792}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>